<commit_message>
Spacing on the latency chart
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Documents\repos\safeplug-audit\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="14136" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="coca-cola" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="google" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -114,6 +119,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -178,25 +191,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.8385</c:v>
+                  <c:v>1.8385000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.448</c:v>
+                  <c:v>5.4480000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.913</c:v>
+                  <c:v>10.912999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.839</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.399499999999999</c:v>
+                  <c:v>5.3994999999999989</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.272</c:v>
+                  <c:v>7.2720000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -211,20 +224,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2124256840"/>
-        <c:axId val="2124262776"/>
+        <c:axId val="203727664"/>
+        <c:axId val="203726880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2124256840"/>
+        <c:axId val="203727664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124262776"/>
+        <c:crossAx val="203726880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -232,7 +246,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124262776"/>
+        <c:axId val="203726880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -243,7 +257,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124256840"/>
+        <c:crossAx val="203727664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -254,7 +268,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -321,22 +335,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.8345</c:v>
+                  <c:v>3.8344999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.913999999999999</c:v>
+                  <c:v>3.9139999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.38000000000001</c:v>
+                  <c:v>26.380000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.10899999999999</c:v>
+                  <c:v>14.108999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.75</c:v>
+                  <c:v>2.7500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.6045</c:v>
+                  <c:v>16.604500000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>13.622</c:v>
@@ -354,20 +368,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2106672808"/>
-        <c:axId val="2107458856"/>
+        <c:axId val="203728448"/>
+        <c:axId val="203729232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2106672808"/>
+        <c:axId val="203728448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107458856"/>
+        <c:crossAx val="203729232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -375,7 +390,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107458856"/>
+        <c:axId val="203729232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -386,7 +401,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106672808"/>
+        <c:crossAx val="203728448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -397,7 +412,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -464,25 +479,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.835</c:v>
+                  <c:v>0.83500000000000019</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8395</c:v>
+                  <c:v>0.83949999999999991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3787</c:v>
+                  <c:v>0.37869999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.069499999999999</c:v>
+                  <c:v>3.0694999999999992</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81345</c:v>
+                  <c:v>0.8134499999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.657000000000001</c:v>
+                  <c:v>3.6570000000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8975</c:v>
+                  <c:v>1.8975000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -497,20 +512,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2127334376"/>
-        <c:axId val="2127427896"/>
+        <c:axId val="203726096"/>
+        <c:axId val="252038896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127334376"/>
+        <c:axId val="203726096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127427896"/>
+        <c:crossAx val="252038896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -518,7 +534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127427896"/>
+        <c:axId val="252038896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,7 +545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127334376"/>
+        <c:crossAx val="203726096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -540,7 +556,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -560,9 +576,43 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Latency Comparison of</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+              <a:t> the Safeplug Settings</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.1317466108390321E-2"/>
+          <c:y val="2.5892070161005993E-2"/>
+          <c:w val="0.90564457480556571"/>
+          <c:h val="0.8587587407450934"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -610,25 +660,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.835</c:v>
+                  <c:v>0.83500000000000019</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8395</c:v>
+                  <c:v>0.83949999999999991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3787</c:v>
+                  <c:v>0.37869999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.069499999999999</c:v>
+                  <c:v>3.0694999999999992</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81345</c:v>
+                  <c:v>0.8134499999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.657000000000001</c:v>
+                  <c:v>3.6570000000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8975</c:v>
+                  <c:v>1.8975000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -677,25 +727,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.8385</c:v>
+                  <c:v>1.8385000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.448</c:v>
+                  <c:v>5.4480000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.913</c:v>
+                  <c:v>10.912999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.839</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.399499999999999</c:v>
+                  <c:v>5.3994999999999989</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.272</c:v>
+                  <c:v>7.2720000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -744,22 +794,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.8345</c:v>
+                  <c:v>3.8344999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.913999999999999</c:v>
+                  <c:v>3.9139999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.38000000000001</c:v>
+                  <c:v>26.380000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.10899999999999</c:v>
+                  <c:v>14.108999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.75</c:v>
+                  <c:v>2.7500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.6045</c:v>
+                  <c:v>16.604500000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>13.622</c:v>
@@ -777,20 +827,50 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2119921080"/>
-        <c:axId val="2119635560"/>
+        <c:axId val="252036936"/>
+        <c:axId val="252039288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2119921080"/>
+        <c:axId val="252036936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Browsing Settings</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119635560"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="252039288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -798,26 +878,81 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119635560"/>
+        <c:axId val="252039288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0"/>
+              <c:y val="0.36855259871900337"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119921080"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="252036936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.76009733261235102"/>
+          <c:y val="0.2175270302033141"/>
+          <c:w val="0.19756964763223975"/>
+          <c:h val="0.12651292014337759"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -825,7 +960,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -940,8 +1075,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>815340</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
@@ -1301,18 +1436,18 @@
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" customWidth="1"/>
+    <col min="2" max="2" width="26.796875" customWidth="1"/>
+    <col min="3" max="3" width="24.296875" customWidth="1"/>
+    <col min="4" max="4" width="22.296875" customWidth="1"/>
+    <col min="5" max="5" width="23.296875" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1335,7 +1470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.93</v>
       </c>
@@ -1358,7 +1493,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.6</v>
       </c>
@@ -1381,7 +1516,7 @@
         <v>9.15</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2.1</v>
       </c>
@@ -1404,7 +1539,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2.67</v>
       </c>
@@ -1427,7 +1562,7 @@
         <v>10.220000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1.61</v>
       </c>
@@ -1450,7 +1585,7 @@
         <v>6.46</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1.41</v>
       </c>
@@ -1473,7 +1608,7 @@
         <v>7.54</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3.25</v>
       </c>
@@ -1496,7 +1631,7 @@
         <v>6.59</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1.46</v>
       </c>
@@ -1519,7 +1654,7 @@
         <v>6.34</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1.81</v>
       </c>
@@ -1542,7 +1677,7 @@
         <v>6.41</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1.26</v>
       </c>
@@ -1565,7 +1700,7 @@
         <v>6.19</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3.47</v>
       </c>
@@ -1588,7 +1723,7 @@
         <v>6.51</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1.61</v>
       </c>
@@ -1611,7 +1746,7 @@
         <v>6.93</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1.54</v>
       </c>
@@ -1634,7 +1769,7 @@
         <v>7.43</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1.43</v>
       </c>
@@ -1657,7 +1792,7 @@
         <v>6.53</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1.66</v>
       </c>
@@ -1680,7 +1815,7 @@
         <v>7.37</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2.72</v>
       </c>
@@ -1703,7 +1838,7 @@
         <v>8.52</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1.25</v>
       </c>
@@ -1726,7 +1861,7 @@
         <v>6.87</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1.25</v>
       </c>
@@ -1749,7 +1884,7 @@
         <v>6.71</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1.24</v>
       </c>
@@ -1772,7 +1907,7 @@
         <v>7.39</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1.5</v>
       </c>
@@ -1795,33 +1930,33 @@
         <v>7.26</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f>AVERAGE(A2:A21)</f>
+        <f t="shared" ref="A23:G23" si="0">AVERAGE(A2:A21)</f>
         <v>1.8385000000000002</v>
       </c>
       <c r="B23">
-        <f>AVERAGE(B2:B21)</f>
+        <f t="shared" si="0"/>
         <v>2.35</v>
       </c>
       <c r="C23">
-        <f>AVERAGE(C2:C21)</f>
+        <f t="shared" si="0"/>
         <v>5.4480000000000004</v>
       </c>
       <c r="D23">
-        <f>AVERAGE(D2:D21)</f>
+        <f t="shared" si="0"/>
         <v>10.912999999999998</v>
       </c>
       <c r="E23">
-        <f>AVERAGE(E2:E21)</f>
+        <f t="shared" si="0"/>
         <v>1.839</v>
       </c>
       <c r="F23">
-        <f>AVERAGE(F2:F21)</f>
+        <f t="shared" si="0"/>
         <v>5.3994999999999989</v>
       </c>
       <c r="G23">
-        <f>AVERAGE(G2:G21)</f>
+        <f t="shared" si="0"/>
         <v>7.2720000000000002</v>
       </c>
     </row>
@@ -1845,18 +1980,18 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.296875" customWidth="1"/>
+    <col min="2" max="2" width="26.19921875" customWidth="1"/>
+    <col min="3" max="3" width="24.296875" customWidth="1"/>
     <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.69921875" customWidth="1"/>
+    <col min="6" max="6" width="31.19921875" customWidth="1"/>
+    <col min="7" max="7" width="18.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1879,7 +2014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4.55</v>
       </c>
@@ -1902,7 +2037,7 @@
         <v>13.95</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4.05</v>
       </c>
@@ -1925,7 +2060,7 @@
         <v>14.07</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3.13</v>
       </c>
@@ -1948,7 +2083,7 @@
         <v>13.02</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7.88</v>
       </c>
@@ -1971,7 +2106,7 @@
         <v>13.73</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3.89</v>
       </c>
@@ -1994,7 +2129,7 @@
         <v>13.83</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5.09</v>
       </c>
@@ -2017,7 +2152,7 @@
         <v>12.72</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4.62</v>
       </c>
@@ -2040,7 +2175,7 @@
         <v>14.09</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3.44</v>
       </c>
@@ -2063,7 +2198,7 @@
         <v>14.82</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3.5</v>
       </c>
@@ -2086,7 +2221,7 @@
         <v>13.96</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3.86</v>
       </c>
@@ -2109,7 +2244,7 @@
         <v>13.19</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2.13</v>
       </c>
@@ -2132,7 +2267,7 @@
         <v>15.05</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2.93</v>
       </c>
@@ -2155,7 +2290,7 @@
         <v>17.84</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3.3</v>
       </c>
@@ -2178,7 +2313,7 @@
         <v>13.73</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4.46</v>
       </c>
@@ -2201,7 +2336,7 @@
         <v>13.14</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3.73</v>
       </c>
@@ -2224,7 +2359,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2.95</v>
       </c>
@@ -2247,7 +2382,7 @@
         <v>12.81</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2.98</v>
       </c>
@@ -2270,7 +2405,7 @@
         <v>11.85</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3.15</v>
       </c>
@@ -2293,7 +2428,7 @@
         <v>12.58</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3.55</v>
       </c>
@@ -2316,7 +2451,7 @@
         <v>12.46</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3.5</v>
       </c>
@@ -2339,33 +2474,33 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f>AVERAGE(A2:A21)</f>
+        <f t="shared" ref="A23:G23" si="0">AVERAGE(A2:A21)</f>
         <v>3.8344999999999998</v>
       </c>
       <c r="B23">
-        <f>AVERAGE(B2:B21)</f>
+        <f t="shared" si="0"/>
         <v>3.9139999999999993</v>
       </c>
       <c r="C23">
-        <f>AVERAGE(C2:C21)</f>
+        <f t="shared" si="0"/>
         <v>26.380000000000006</v>
       </c>
       <c r="D23">
-        <f>AVERAGE(D2:D21)</f>
+        <f t="shared" si="0"/>
         <v>14.108999999999995</v>
       </c>
       <c r="E23">
-        <f>AVERAGE(E2:E21)</f>
+        <f t="shared" si="0"/>
         <v>2.7500000000000004</v>
       </c>
       <c r="F23">
-        <f>AVERAGE(F2:F21)</f>
+        <f t="shared" si="0"/>
         <v>16.604500000000002</v>
       </c>
       <c r="G23">
-        <f>AVERAGE(G2:G21)</f>
+        <f t="shared" si="0"/>
         <v>13.622</v>
       </c>
     </row>
@@ -2388,18 +2523,18 @@
       <selection activeCell="A23" activeCellId="1" sqref="A1:XFD1 A23:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.296875" customWidth="1"/>
+    <col min="2" max="2" width="26.796875" customWidth="1"/>
+    <col min="3" max="3" width="24.19921875" customWidth="1"/>
+    <col min="4" max="4" width="22.19921875" customWidth="1"/>
+    <col min="5" max="5" width="24.69921875" customWidth="1"/>
     <col min="6" max="6" width="31.5" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2422,7 +2557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.83899999999999997</v>
       </c>
@@ -2445,7 +2580,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.82399999999999995</v>
       </c>
@@ -2468,7 +2603,7 @@
         <v>2.04</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.77600000000000002</v>
       </c>
@@ -2491,7 +2626,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.78600000000000003</v>
       </c>
@@ -2514,7 +2649,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1.03</v>
       </c>
@@ -2537,7 +2672,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.79100000000000004</v>
       </c>
@@ -2560,7 +2695,7 @@
         <v>1.89</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.80900000000000005</v>
       </c>
@@ -2583,7 +2718,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.85299999999999998</v>
       </c>
@@ -2606,7 +2741,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.80600000000000005</v>
       </c>
@@ -2629,7 +2764,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.78100000000000003</v>
       </c>
@@ -2652,7 +2787,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.86899999999999999</v>
       </c>
@@ -2675,7 +2810,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0.77900000000000003</v>
       </c>
@@ -2698,7 +2833,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0.97299999999999998</v>
       </c>
@@ -2721,7 +2856,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0.90900000000000003</v>
       </c>
@@ -2744,7 +2879,7 @@
         <v>1.93</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0.77200000000000002</v>
       </c>
@@ -2767,7 +2902,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0.79700000000000004</v>
       </c>
@@ -2790,7 +2925,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0.86099999999999999</v>
       </c>
@@ -2813,7 +2948,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0.78300000000000003</v>
       </c>
@@ -2836,7 +2971,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0.80200000000000005</v>
       </c>
@@ -2859,7 +2994,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0.86</v>
       </c>
@@ -2882,33 +3017,33 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f>AVERAGE(A2:A21)</f>
+        <f t="shared" ref="A23:G23" si="0">AVERAGE(A2:A21)</f>
         <v>0.83500000000000019</v>
       </c>
       <c r="B23">
-        <f>AVERAGE(B2:B21)</f>
+        <f t="shared" si="0"/>
         <v>0.83949999999999991</v>
       </c>
       <c r="C23">
-        <f>AVERAGE(C2:C21)</f>
+        <f t="shared" si="0"/>
         <v>0.37869999999999998</v>
       </c>
       <c r="D23">
-        <f>AVERAGE(D2:D21)</f>
+        <f t="shared" si="0"/>
         <v>3.0694999999999992</v>
       </c>
       <c r="E23">
-        <f>AVERAGE(E2:E21)</f>
+        <f t="shared" si="0"/>
         <v>0.8134499999999999</v>
       </c>
       <c r="F23">
-        <f>AVERAGE(F2:F21)</f>
+        <f t="shared" si="0"/>
         <v>3.6570000000000009</v>
       </c>
       <c r="G23">
-        <f>AVERAGE(G2:G21)</f>
+        <f t="shared" si="0"/>
         <v>1.8975000000000002</v>
       </c>
     </row>
@@ -2927,9 +3062,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
still trying to make new graph
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="coca-cola" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="7">
   <si>
     <t>Plain Firefox</t>
   </si>
@@ -92,8 +92,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -104,13 +110,19 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -212,11 +224,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2101453096"/>
-        <c:axId val="2101456104"/>
+        <c:axId val="2067542984"/>
+        <c:axId val="2067545992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2101453096"/>
+        <c:axId val="2067542984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -225,7 +237,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101456104"/>
+        <c:crossAx val="2067545992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -233,7 +245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101456104"/>
+        <c:axId val="2067545992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -244,7 +256,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101453096"/>
+        <c:crossAx val="2067542984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -275,6 +287,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -283,64 +299,252 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>washingtonpost!$A$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Plain Firefox</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Firefox, no tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Firefox, tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Firefox, tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Firefox, no tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Tor Browser Bundle with Safeplug</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Tor Browser Bundle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>washingtonpost!$A$23:$G$23</c:f>
+              <c:f>'coca-cola'!$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3.8345</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.913999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26.38000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.10899999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16.6045</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13.622</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.8385</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.448</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10.913</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.839</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$F$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.399499999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,11 +559,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2106990888"/>
-        <c:axId val="2106993896"/>
+        <c:axId val="2080457528"/>
+        <c:axId val="2080460920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2106990888"/>
+        <c:axId val="2080457528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -368,7 +572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106993896"/>
+        <c:crossAx val="2080460920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -376,7 +580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106993896"/>
+        <c:axId val="2080460920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,11 +591,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106990888"/>
+        <c:crossAx val="2080457528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -431,7 +640,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>google!$A$1:$G$1</c:f>
+              <c:f>washingtonpost!$A$1:$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -460,30 +669,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>google!$A$23:$G$23</c:f>
+              <c:f>washingtonpost!$A$23:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.835</c:v>
+                  <c:v>3.8345</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8395</c:v>
+                  <c:v>3.913999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3787</c:v>
+                  <c:v>26.38000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.069499999999999</c:v>
+                  <c:v>14.10899999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81345</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.657000000000001</c:v>
+                  <c:v>16.6045</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8975</c:v>
+                  <c:v>13.622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -498,11 +707,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2107429144"/>
-        <c:axId val="2107432152"/>
+        <c:axId val="2067610504"/>
+        <c:axId val="2067613512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2107429144"/>
+        <c:axId val="2067610504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -511,7 +720,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107432152"/>
+        <c:crossAx val="2067613512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -519,7 +728,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107432152"/>
+        <c:axId val="2067613512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +739,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107429144"/>
+        <c:crossAx val="2067610504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -548,6 +757,829 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.8345</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.913999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>26.38000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>14.10899999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$F$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16.6045</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>13.622</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2098294856"/>
+        <c:axId val="2101039912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2098294856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2101039912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2101039912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2098294856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>google!$A$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$A$23:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.835</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8395</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3787</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.069499999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81345</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.657000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8975</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2051200360"/>
+        <c:axId val="2051150328"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2051200360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2051150328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2051150328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2051200360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.8395</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.3787</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.069499999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.81345</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$F$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.657000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.8975</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2100101048"/>
+        <c:axId val="2100104472"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2100101048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2100104472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2100104472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2100101048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -802,11 +1834,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2107476472"/>
-        <c:axId val="2107481944"/>
+        <c:axId val="2067646952"/>
+        <c:axId val="2067653624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2107476472"/>
+        <c:axId val="2067646952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -834,7 +1866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107481944"/>
+        <c:crossAx val="2067653624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -842,7 +1874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107481944"/>
+        <c:axId val="2067653624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,7 +1904,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107476472"/>
+        <c:crossAx val="2067646952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -894,7 +1926,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -908,6 +1940,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -916,128 +1952,255 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Plain Firefox</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>(google!$A$23,google!$A$23)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.835</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.835</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Firefox, no Tor, no ad-blocking</c:v>
+            <c:strRef>
+              <c:f>'coca-cola'!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
+          <c:cat>
+            <c:strLit>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1.0</c:v>
+                <c:v>_x0011_www.coca-cola.com</c:v>
               </c:pt>
-            </c:numLit>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.8385</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Firefox, Tor, no ad-blocking</c:v>
+            <c:strRef>
+              <c:f>'coca-cola'!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
+          <c:cat>
+            <c:strLit>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1.0</c:v>
+                <c:v>_x0011_www.coca-cola.com</c:v>
               </c:pt>
-            </c:numLit>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Firefox, Tor, ad-blocking</c:v>
+            <c:strRef>
+              <c:f>'coca-cola'!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
+          <c:cat>
+            <c:strLit>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1.0</c:v>
+                <c:v>_x0011_www.coca-cola.com</c:v>
               </c:pt>
-            </c:numLit>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.448</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>Firefox, no Tor, ad-blocking</c:v>
+            <c:strRef>
+              <c:f>'coca-cola'!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
+          <c:cat>
+            <c:strLit>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1.0</c:v>
+                <c:v>_x0011_www.coca-cola.com</c:v>
               </c:pt>
-            </c:numLit>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10.913</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>Tor Browser Bundle with Safeplug</c:v>
+            <c:strRef>
+              <c:f>'coca-cola'!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
+          <c:cat>
+            <c:strLit>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1.0</c:v>
+                <c:v>_x0011_www.coca-cola.com</c:v>
               </c:pt>
-            </c:numLit>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.839</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>Tor Browser Bundle</c:v>
+            <c:strRef>
+              <c:f>'coca-cola'!$F$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
+          <c:cat>
+            <c:strLit>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1.0</c:v>
+                <c:v>_x0011_www.coca-cola.com</c:v>
               </c:pt>
-            </c:numLit>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.399499999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.272</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
@@ -1049,11 +2212,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2098396040"/>
-        <c:axId val="2108978200"/>
+        <c:axId val="2087572824"/>
+        <c:axId val="2073078168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2098396040"/>
+        <c:axId val="2087572824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1062,7 +2225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108978200"/>
+        <c:crossAx val="2073078168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1070,7 +2233,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108978200"/>
+        <c:axId val="2073078168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1081,7 +2244,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2098396040"/>
+        <c:crossAx val="2087572824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1135,6 +2298,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1130300</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1170,6 +2363,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1308100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1200,6 +2423,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2032000</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1249,21 +2502,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1604,8 +2859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2102,6 +3357,29 @@
         <v>7.26</v>
       </c>
     </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="23" spans="1:7">
       <c r="A23">
         <f t="shared" ref="A23:G23" si="0">AVERAGE(A2:A21)</f>
@@ -2148,8 +3426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2646,6 +3924,29 @@
         <v>12.5</v>
       </c>
     </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="23" spans="1:7">
       <c r="A23">
         <f t="shared" ref="A23:G23" si="0">AVERAGE(A2:A21)</f>
@@ -2691,8 +3992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A23" activeCellId="1" sqref="A1:XFD1 A23:XFD23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3166,7 +4467,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="16" customHeight="1">
       <c r="A21">
         <v>0.86</v>
       </c>
@@ -3187,6 +4488,29 @@
       </c>
       <c r="G21">
         <v>1.94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3221,6 +4545,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3234,8 +4559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3254,7 +4579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
made changes to figure, graph, arrangement
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="15">
   <si>
     <t>Plain Firefox</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Firefox, no Tor, ad-blocking</t>
+  </si>
+  <si>
+    <t>Average Among the 3 Sites</t>
   </si>
 </sst>
 </file>
@@ -255,11 +258,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099696728"/>
-        <c:axId val="2099308280"/>
+        <c:axId val="2099489944"/>
+        <c:axId val="2099486920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099696728"/>
+        <c:axId val="2099489944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -268,7 +271,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099308280"/>
+        <c:crossAx val="2099486920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -276,7 +279,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099308280"/>
+        <c:axId val="2099486920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -287,7 +290,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099696728"/>
+        <c:crossAx val="2099489944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -319,7 +322,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -590,11 +592,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099362680"/>
-        <c:axId val="2100175960"/>
+        <c:axId val="2099405688"/>
+        <c:axId val="2099402696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099362680"/>
+        <c:axId val="2099405688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +605,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100175960"/>
+        <c:crossAx val="2099402696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -611,7 +613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100175960"/>
+        <c:axId val="2099402696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -622,14 +624,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099362680"/>
+        <c:crossAx val="2099405688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -738,11 +739,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2066840792"/>
-        <c:axId val="2103155560"/>
+        <c:axId val="2099374088"/>
+        <c:axId val="2099371064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2066840792"/>
+        <c:axId val="2099374088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +752,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103155560"/>
+        <c:crossAx val="2099371064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,7 +760,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2103155560"/>
+        <c:axId val="2099371064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +771,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066840792"/>
+        <c:crossAx val="2099374088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -802,7 +803,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1073,11 +1073,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2066222792"/>
-        <c:axId val="2067261576"/>
+        <c:axId val="2099321416"/>
+        <c:axId val="2099318424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2066222792"/>
+        <c:axId val="2099321416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1086,7 +1086,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067261576"/>
+        <c:crossAx val="2099318424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1094,7 +1094,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2067261576"/>
+        <c:axId val="2099318424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1105,14 +1105,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066222792"/>
+        <c:crossAx val="2099321416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1221,11 +1220,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2066256664"/>
-        <c:axId val="2066259672"/>
+        <c:axId val="2099291144"/>
+        <c:axId val="2099288120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2066256664"/>
+        <c:axId val="2099291144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1234,7 +1233,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066259672"/>
+        <c:crossAx val="2099288120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1242,7 +1241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2066259672"/>
+        <c:axId val="2099288120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1253,7 +1252,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066256664"/>
+        <c:crossAx val="2099291144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1285,7 +1284,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1556,11 +1554,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2065828312"/>
-        <c:axId val="2065824712"/>
+        <c:axId val="2100672024"/>
+        <c:axId val="2100675000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2065828312"/>
+        <c:axId val="2100672024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1569,7 +1567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065824712"/>
+        <c:crossAx val="2100675000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1577,7 +1575,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2065824712"/>
+        <c:axId val="2100675000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1588,14 +1586,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065828312"/>
+        <c:crossAx val="2100672024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1645,7 +1642,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1865,11 +1861,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2066384664"/>
-        <c:axId val="2099858440"/>
+        <c:axId val="2100715240"/>
+        <c:axId val="2100720664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2066384664"/>
+        <c:axId val="2100715240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1891,13 +1887,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099858440"/>
+        <c:crossAx val="2100720664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1905,7 +1900,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099858440"/>
+        <c:axId val="2100720664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1928,21 +1923,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066384664"/>
+        <c:crossAx val="2100715240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1972,7 +1965,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2243,11 +2235,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2103744712"/>
-        <c:axId val="2103747688"/>
+        <c:axId val="2100778248"/>
+        <c:axId val="2100781224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2103744712"/>
+        <c:axId val="2100778248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,7 +2248,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103747688"/>
+        <c:crossAx val="2100781224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2264,7 +2256,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2103747688"/>
+        <c:axId val="2100781224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2275,14 +2267,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103744712"/>
+        <c:crossAx val="2100778248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2354,9 +2345,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$B$7:$D$7</c:f>
+              <c:f>Sheet3!$B$7:$E$7</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>www.coca-cola.com</c:v>
                 </c:pt>
@@ -2365,16 +2356,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>www.google.com</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Average Among the 3 Sites</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$8:$D$8</c:f>
+              <c:f>Sheet3!$B$8:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1.8385</c:v>
                 </c:pt>
@@ -2383,6 +2377,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.835</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1693</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2405,9 +2402,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$B$7:$D$7</c:f>
+              <c:f>Sheet3!$B$7:$E$7</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>www.coca-cola.com</c:v>
                 </c:pt>
@@ -2416,16 +2413,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>www.google.com</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Average Among the 3 Sites</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$9:$D$9</c:f>
+              <c:f>Sheet3!$B$9:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>2.35</c:v>
                 </c:pt>
@@ -2434,6 +2434,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.8395</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2456,9 +2459,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$B$7:$D$7</c:f>
+              <c:f>Sheet3!$B$7:$E$7</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>www.coca-cola.com</c:v>
                 </c:pt>
@@ -2467,16 +2470,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>www.google.com</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Average Among the 3 Sites</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$10:$D$10</c:f>
+              <c:f>Sheet3!$B$10:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5.448</c:v>
                 </c:pt>
@@ -2485,6 +2491,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.3787</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.7356</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2507,9 +2516,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$B$7:$D$7</c:f>
+              <c:f>Sheet3!$B$7:$E$7</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>www.coca-cola.com</c:v>
                 </c:pt>
@@ -2518,16 +2527,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>www.google.com</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Average Among the 3 Sites</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$11:$D$11</c:f>
+              <c:f>Sheet3!$B$11:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>10.913</c:v>
                 </c:pt>
@@ -2536,6 +2548,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.0695</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3638</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2558,9 +2573,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$B$7:$D$7</c:f>
+              <c:f>Sheet3!$B$7:$E$7</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>www.coca-cola.com</c:v>
                 </c:pt>
@@ -2569,16 +2584,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>www.google.com</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Average Among the 3 Sites</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$12:$D$12</c:f>
+              <c:f>Sheet3!$B$12:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1.839</c:v>
                 </c:pt>
@@ -2587,6 +2605,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.81345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2609,9 +2630,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$B$7:$D$7</c:f>
+              <c:f>Sheet3!$B$7:$E$7</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>www.coca-cola.com</c:v>
                 </c:pt>
@@ -2620,16 +2641,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>www.google.com</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Average Among the 3 Sites</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$13:$D$13</c:f>
+              <c:f>Sheet3!$B$13:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5.3995</c:v>
                 </c:pt>
@@ -2638,6 +2662,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.657</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.5537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2660,9 +2687,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$B$7:$D$7</c:f>
+              <c:f>Sheet3!$B$7:$E$7</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>www.coca-cola.com</c:v>
                 </c:pt>
@@ -2671,16 +2698,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>www.google.com</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Average Among the 3 Sites</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$14:$D$14</c:f>
+              <c:f>Sheet3!$B$14:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>7.272</c:v>
                 </c:pt>
@@ -2689,6 +2719,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.8975</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2703,11 +2736,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105168936"/>
-        <c:axId val="2051299144"/>
+        <c:axId val="2100838808"/>
+        <c:axId val="2100844168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105168936"/>
+        <c:axId val="2100838808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2735,7 +2768,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2051299144"/>
+        <c:crossAx val="2100844168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2743,7 +2776,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2051299144"/>
+        <c:axId val="2100844168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2773,7 +2806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105168936"/>
+        <c:crossAx val="2100838808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5164,7 +5197,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5290,6 +5323,9 @@
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -5304,6 +5340,9 @@
       <c r="D8">
         <v>0.83499999999999996</v>
       </c>
+      <c r="E8">
+        <v>2.1692999999999998</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -5318,6 +5357,9 @@
       <c r="D9">
         <v>0.83950000000000002</v>
       </c>
+      <c r="E9">
+        <v>2.3677999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
@@ -5332,6 +5374,9 @@
       <c r="D10">
         <v>0.37869999999999998</v>
       </c>
+      <c r="E10">
+        <v>10.7356</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
@@ -5346,6 +5391,9 @@
       <c r="D11">
         <v>3.0695000000000001</v>
       </c>
+      <c r="E11">
+        <v>9.3637999999999995</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -5360,6 +5408,9 @@
       <c r="D12">
         <v>0.81345000000000001</v>
       </c>
+      <c r="E12">
+        <v>1.8008</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -5374,6 +5425,9 @@
       <c r="D13">
         <v>3.657</v>
       </c>
+      <c r="E13">
+        <v>8.5536999999999992</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -5387,6 +5441,9 @@
       </c>
       <c r="D14">
         <v>1.8975</v>
+      </c>
+      <c r="E14">
+        <v>7.5972</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new plot for measurements, new edits
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="coca-cola" sheetId="1" r:id="rId1"/>
@@ -258,11 +258,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099489944"/>
-        <c:axId val="2099486920"/>
+        <c:axId val="2068190600"/>
+        <c:axId val="2068193608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099489944"/>
+        <c:axId val="2068190600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -271,7 +271,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099486920"/>
+        <c:crossAx val="2068193608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -279,7 +279,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099486920"/>
+        <c:axId val="2068193608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -290,7 +290,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099489944"/>
+        <c:crossAx val="2068190600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -307,1988 +307,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$A$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Plain Firefox</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.8385</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$B$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, no tor, no ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$B$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2.35</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$C$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, tor, no ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$C$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5.448</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$D$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, tor, ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$D$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10.913</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$E$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, no tor, ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$E$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.839</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$F$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tor Browser Bundle with Safeplug</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$F$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5.399499999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$G$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tor Browser Bundle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$G$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>7.272</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2099405688"/>
-        <c:axId val="2099402696"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2099405688"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099402696"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2099402696"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099405688"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>washingtonpost!$A$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Plain Firefox</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Firefox, no tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Firefox, tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Firefox, tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Firefox, no tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Tor Browser Bundle with Safeplug</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Tor Browser Bundle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>washingtonpost!$A$23:$G$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3.8345</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.913999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26.38000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.10899999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16.6045</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13.622</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2099374088"/>
-        <c:axId val="2099371064"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2099374088"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099371064"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2099371064"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099374088"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>washingtonpost!$A$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Plain Firefox</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0016_www.washingtonpost.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>washingtonpost!$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3.8345</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>washingtonpost!$B$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, no tor, no ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0016_www.washingtonpost.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>washingtonpost!$B$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3.913999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>washingtonpost!$C$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, tor, no ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0016_www.washingtonpost.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>washingtonpost!$C$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>26.38000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>washingtonpost!$D$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, tor, ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0016_www.washingtonpost.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>washingtonpost!$D$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>14.10899999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>washingtonpost!$E$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, no tor, ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0016_www.washingtonpost.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>washingtonpost!$E$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>washingtonpost!$F$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tor Browser Bundle with Safeplug</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0016_www.washingtonpost.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>washingtonpost!$F$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>16.6045</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>washingtonpost!$G$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tor Browser Bundle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0016_www.washingtonpost.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>washingtonpost!$G$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>13.622</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2099321416"/>
-        <c:axId val="2099318424"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2099321416"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099318424"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2099318424"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099321416"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>google!$A$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Plain Firefox</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Firefox, no tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Firefox, tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Firefox, tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Firefox, no tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Tor Browser Bundle with Safeplug</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Tor Browser Bundle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>google!$A$23:$G$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.835</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.8395</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.3787</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.069499999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.81345</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.657000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.8975</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2099291144"/>
-        <c:axId val="2099288120"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2099291144"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099288120"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2099288120"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099291144"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>google!$A$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Plain Firefox</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x000e_www.google.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>google!$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.835</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>google!$B$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, no tor, no ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x000e_www.google.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>google!$B$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.8395</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>google!$C$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, tor, no ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x000e_www.google.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>google!$C$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.3787</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>google!$D$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, tor, ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x000e_www.google.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>google!$D$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3.069499999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>google!$E$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, no tor, ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x000e_www.google.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>google!$E$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.81345</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>google!$F$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tor Browser Bundle with Safeplug</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x000e_www.google.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>google!$F$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3.657000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>google!$G$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tor Browser Bundle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x000e_www.google.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>google!$G$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.8975</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2100672024"/>
-        <c:axId val="2100675000"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2100672024"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100675000"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2100675000"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100672024"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Latency Comparison</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of the Safeplug</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>www.google.com</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>google!$A$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Plain Firefox</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Firefox, no tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Firefox, tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Firefox, tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Firefox, no tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Tor Browser Bundle with Safeplug</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Tor Browser Bundle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>google!$A$23:$G$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.835</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.8395</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.3787</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.069499999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.81345</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.657000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.8975</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>www.coca-cola.com</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'coca-cola'!$A$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Plain Firefox</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Firefox, no tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Firefox, tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Firefox, tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Firefox, no tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Tor Browser Bundle with Safeplug</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Tor Browser Bundle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$A$23:$G$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.8385</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.35</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.448</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.913</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.839</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.399499999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.272</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>www.washingtonpost.com</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>washingtonpost!$A$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Plain Firefox</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Firefox, no tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Firefox, tor, no ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Firefox, tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Firefox, no tor, ad-blocking</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Tor Browser Bundle with Safeplug</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Tor Browser Bundle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>washingtonpost!$A$23:$G$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3.8345</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.913999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26.38000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.10899999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16.6045</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13.622</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2100715240"/>
-        <c:axId val="2100720664"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2100715240"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Platform</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100720664"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2100720664"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time (seconds)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100715240"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$A$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Plain Firefox</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.8385</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$B$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, no tor, no ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$B$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2.35</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$C$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, tor, no ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$C$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5.448</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$D$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, tor, ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$D$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10.913</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$E$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox, no tor, ad-blocking</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$E$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.839</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$F$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tor Browser Bundle with Safeplug</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$F$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5.399499999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'coca-cola'!$G$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tor Browser Bundle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0011_www.coca-cola.com</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'coca-cola'!$G$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>7.272</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2100778248"/>
-        <c:axId val="2100781224"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2100778248"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100781224"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2100781224"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100778248"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2736,11 +755,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2100838808"/>
-        <c:axId val="2100844168"/>
+        <c:axId val="2068538360"/>
+        <c:axId val="2068543720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2100838808"/>
+        <c:axId val="2068538360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2768,7 +787,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100844168"/>
+        <c:crossAx val="2068543720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2776,7 +795,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100844168"/>
+        <c:axId val="2068543720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2806,7 +825,2444 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100838808"/>
+        <c:crossAx val="2068538360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.8385</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.448</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10.913</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.839</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$F$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.399499999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.272</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2067232776"/>
+        <c:axId val="2067235752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2067232776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2067235752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2067235752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2067232776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Range and Distribution of Web</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Page Request Time for www.coca-cola.com</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'coca-cola'!$A$31:$G$31</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.185</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.3825</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3.245</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.2175</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.2175</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'coca-cola'!$A$22:$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$A$32:$G$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.425</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9225</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.145</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5975</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'coca-cola'!$A$22:$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$A$33:$G$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4525</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.145</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.465000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.489999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="plus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'coca-cola'!$A$35:$G$35</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>1.4975</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.265</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.31</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.404999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.225</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.09</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.762500000000001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'coca-cola'!$A$22:$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$A$34:$G$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.3675</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.095000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.244999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4425</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="2082117176"/>
+        <c:axId val="2080525016"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2082117176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Setting</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2080525016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2080525016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2082117176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>washingtonpost!$A$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$A$23:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.8345</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.913999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.38000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.10899999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.6045</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.622</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2068280744"/>
+        <c:axId val="2068283752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2068280744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068283752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2068283752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068280744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.8345</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.913999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>26.38000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>14.10899999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$F$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16.6045</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>washingtonpost!$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0016_www.washingtonpost.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>13.622</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2068336824"/>
+        <c:axId val="2068339800"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2068336824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068339800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2068339800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068336824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>google!$A$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$A$23:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.835</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8395</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3787</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.069499999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81345</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.657000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8975</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2068367176"/>
+        <c:axId val="2068370184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2068367176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068370184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2068370184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068367176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.8395</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.3787</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.069499999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.81345</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$F$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.657000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>google!$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x000e_www.google.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.8975</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2068420120"/>
+        <c:axId val="2068423096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2068420120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068423096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2068423096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068420120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Latency Comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of the Safeplug</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>www.google.com</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>google!$A$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>google!$A$23:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.835</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8395</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3787</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.069499999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81345</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.657000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8975</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>www.coca-cola.com</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'coca-cola'!$A$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$A$23:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.8385</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.448</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.913</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.839</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.399499999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.272</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>www.washingtonpost.com</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>washingtonpost!$A$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>washingtonpost!$A$23:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.8345</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.913999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.38000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.10899999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.6045</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.622</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2067263096"/>
+        <c:axId val="2067268520"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2067263096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Platform</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2067268520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2067268520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2067263096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Firefox</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.8385</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, no ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.448</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10.913</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox, no tor, ad-blocking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.839</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$F$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle with Safeplug</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.399499999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coca-cola'!$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tor Browser Bundle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0011_www.coca-cola.com</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coca-cola'!$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.272</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2068464872"/>
+        <c:axId val="2068467848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2068464872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068467848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2068467848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068464872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2832,16 +3288,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1460500</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2862,16 +3318,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1130300</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2885,6 +3341,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>977900</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3454,10 +3940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:G23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4005,6 +4491,306 @@
       <c r="G23">
         <f t="shared" si="0"/>
         <v>7.2720000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <f>MIN(A2:A21)</f>
+        <v>1.24</v>
+      </c>
+      <c r="B25">
+        <f>MIN(B2:B21)</f>
+        <v>1.54</v>
+      </c>
+      <c r="C25">
+        <f>MIN(C2:C21)</f>
+        <v>4.32</v>
+      </c>
+      <c r="D25">
+        <f>MIN(D2:D21)</f>
+        <v>5.9</v>
+      </c>
+      <c r="E25">
+        <f>MIN(E2:E21)</f>
+        <v>1.38</v>
+      </c>
+      <c r="F25">
+        <f>MIN(F2:F21)</f>
+        <v>4.18</v>
+      </c>
+      <c r="G25">
+        <f>MIN(G2:G21)</f>
+        <v>6.19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <f>_xlfn.QUARTILE.INC(A2:A21,1)</f>
+        <v>1.4249999999999998</v>
+      </c>
+      <c r="B26">
+        <f>_xlfn.QUARTILE.INC(B2:B21,1)</f>
+        <v>1.9224999999999999</v>
+      </c>
+      <c r="C26">
+        <f>_xlfn.QUARTILE.INC(C2:C21,1)</f>
+        <v>4.62</v>
+      </c>
+      <c r="D26">
+        <f>_xlfn.QUARTILE.INC(D2:D21,1)</f>
+        <v>9.1449999999999996</v>
+      </c>
+      <c r="E26">
+        <f>_xlfn.QUARTILE.INC(E2:E21,1)</f>
+        <v>1.5975000000000001</v>
+      </c>
+      <c r="F26">
+        <f>_xlfn.QUARTILE.INC(F2:F21,1)</f>
+        <v>4.4799999999999995</v>
+      </c>
+      <c r="G26">
+        <f>_xlfn.QUARTILE.INC(G2:G21,1)</f>
+        <v>6.5250000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <f>MEDIAN(A2:A21)</f>
+        <v>1.605</v>
+      </c>
+      <c r="B27">
+        <f>MEDIAN(B2:B21)</f>
+        <v>2.375</v>
+      </c>
+      <c r="C27">
+        <f>MEDIAN(C2:C21)</f>
+        <v>4.91</v>
+      </c>
+      <c r="D27">
+        <f>MEDIAN(D2:D21)</f>
+        <v>10.29</v>
+      </c>
+      <c r="E27">
+        <f>MEDIAN(E2:E21)</f>
+        <v>1.8050000000000002</v>
+      </c>
+      <c r="F27">
+        <f>MEDIAN(F2:F21)</f>
+        <v>4.9450000000000003</v>
+      </c>
+      <c r="G27">
+        <f>MEDIAN(G2:G21)</f>
+        <v>7.0149999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <f>_xlfn.QUARTILE.INC(A2:A21,3)</f>
+        <v>1.9724999999999999</v>
+      </c>
+      <c r="B28">
+        <f>_xlfn.QUARTILE.INC(B2:B21,3)</f>
+        <v>2.6149999999999998</v>
+      </c>
+      <c r="C28">
+        <f>_xlfn.QUARTILE.INC(C2:C21,3)</f>
+        <v>5.87</v>
+      </c>
+      <c r="D28">
+        <f>_xlfn.QUARTILE.INC(D2:D21,3)</f>
+        <v>12.385</v>
+      </c>
+      <c r="E28">
+        <f>_xlfn.QUARTILE.INC(E2:E21,3)</f>
+        <v>2.105</v>
+      </c>
+      <c r="F28">
+        <f>_xlfn.QUARTILE.INC(F2:F21,3)</f>
+        <v>5.1899999999999995</v>
+      </c>
+      <c r="G28">
+        <f>_xlfn.QUARTILE.INC(G2:G21,3)</f>
+        <v>7.4574999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <f>MAX(A2:A21)</f>
+        <v>3.47</v>
+      </c>
+      <c r="B29">
+        <f>MAX(B2:B21)</f>
+        <v>3.88</v>
+      </c>
+      <c r="C29">
+        <f>MAX(C2:C21)</f>
+        <v>9.18</v>
+      </c>
+      <c r="D29">
+        <f>MAX(D2:D21)</f>
+        <v>19.79</v>
+      </c>
+      <c r="E29">
+        <f>MAX(E2:E21)</f>
+        <v>2.33</v>
+      </c>
+      <c r="F29">
+        <f>MAX(F2:F21)</f>
+        <v>10.28</v>
+      </c>
+      <c r="G29">
+        <f>MAX(G2:G21)</f>
+        <v>10.220000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <f>A26-A25</f>
+        <v>0.18499999999999983</v>
+      </c>
+      <c r="B31">
+        <f>B26-B25</f>
+        <v>0.38249999999999984</v>
+      </c>
+      <c r="C31">
+        <f>C26-C25</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="D31">
+        <f>D26-D25</f>
+        <v>3.2449999999999992</v>
+      </c>
+      <c r="E31">
+        <f>E26-E25</f>
+        <v>0.21750000000000025</v>
+      </c>
+      <c r="F31">
+        <f>F26-F25</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="G31">
+        <f>E26-E25</f>
+        <v>0.21750000000000025</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <f>A26</f>
+        <v>1.4249999999999998</v>
+      </c>
+      <c r="B32">
+        <f>B26</f>
+        <v>1.9224999999999999</v>
+      </c>
+      <c r="C32">
+        <f>C26</f>
+        <v>4.62</v>
+      </c>
+      <c r="D32">
+        <f>D26</f>
+        <v>9.1449999999999996</v>
+      </c>
+      <c r="E32">
+        <f>E26</f>
+        <v>1.5975000000000001</v>
+      </c>
+      <c r="F32">
+        <f>F26</f>
+        <v>4.4799999999999995</v>
+      </c>
+      <c r="G32">
+        <f>G26</f>
+        <v>6.5250000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <f>A27-A26</f>
+        <v>0.18000000000000016</v>
+      </c>
+      <c r="B33">
+        <f>B27-B26</f>
+        <v>0.45250000000000012</v>
+      </c>
+      <c r="C33">
+        <f>C27-C26</f>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="D33">
+        <f>D27-D26</f>
+        <v>1.1449999999999996</v>
+      </c>
+      <c r="E33">
+        <f>E27-E26</f>
+        <v>0.20750000000000002</v>
+      </c>
+      <c r="F33">
+        <f>F27-F26</f>
+        <v>0.46500000000000075</v>
+      </c>
+      <c r="G33">
+        <f>G27-G26</f>
+        <v>0.48999999999999932</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <f>A28-A27</f>
+        <v>0.36749999999999994</v>
+      </c>
+      <c r="B34">
+        <f>B28-B27</f>
+        <v>0.23999999999999977</v>
+      </c>
+      <c r="C34">
+        <f>C28-C27</f>
+        <v>0.96</v>
+      </c>
+      <c r="D34">
+        <f>D28-D27</f>
+        <v>2.0950000000000006</v>
+      </c>
+      <c r="E34">
+        <f>E28-E27</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="F34">
+        <f>F28-F27</f>
+        <v>0.24499999999999922</v>
+      </c>
+      <c r="G34">
+        <f>G28-G27</f>
+        <v>0.44249999999999989</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <f>A29-A28</f>
+        <v>1.4975000000000003</v>
+      </c>
+      <c r="B35">
+        <f>B29-B28</f>
+        <v>1.2650000000000001</v>
+      </c>
+      <c r="C35">
+        <f>C29-C28</f>
+        <v>3.3099999999999996</v>
+      </c>
+      <c r="D35">
+        <f>D29-D28</f>
+        <v>7.4049999999999994</v>
+      </c>
+      <c r="E35">
+        <f>E29-E28</f>
+        <v>0.22500000000000009</v>
+      </c>
+      <c r="F35">
+        <f>F29-F28</f>
+        <v>5.09</v>
+      </c>
+      <c r="G35">
+        <f>G29-G28</f>
+        <v>2.7625000000000011</v>
       </c>
     </row>
   </sheetData>
@@ -5196,7 +5982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>